<commit_message>
Finalizei a aula 3
</commit_message>
<xml_diff>
--- a/Excel VBA/Aula 3 - Cálculos Básicos/Produtos.xlsx
+++ b/Excel VBA/Aula 3 - Cálculos Básicos/Produtos.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Users\bruno\Documents\GitHub\Alura\Excel VBA\Aula 2 - Formatando Passo a Passo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Users\bruno\Documents\GitHub\Alura\Excel VBA\Aula 3 - Cálculos Básicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B927A2F-5002-460D-997E-51B89ECFA28F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB945D6-847A-4F56-AD5D-17FEA97F4FC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{F429CDF2-33A2-4A6E-9034-27FA88637C5A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{F429CDF2-33A2-4A6E-9034-27FA88637C5A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Produtos Adultos" sheetId="3" r:id="rId1"/>
+    <sheet name="Produtos Infantis" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>Tênis Infantil Vermelho</t>
   </si>
@@ -61,6 +62,24 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Lista de Produtos Infantis</t>
+  </si>
+  <si>
+    <t>Quantidades</t>
+  </si>
+  <si>
+    <t>Preço Unitário</t>
+  </si>
+  <si>
+    <t>Valor Total</t>
+  </si>
+  <si>
+    <t>Desconto</t>
+  </si>
+  <si>
+    <t>Valor do desconto</t>
   </si>
 </sst>
 </file>
@@ -70,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,8 +133,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,6 +159,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -280,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -309,6 +340,21 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -318,23 +364,23 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="9" fontId="6" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -650,11 +696,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6CF0F7-701F-4AD3-A160-66200CB65652}">
-  <dimension ref="A1:C20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861A2F3F-23EB-4750-836E-E1F54A5CF7DF}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,11 +712,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="17"/>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -679,211 +725,402 @@
       <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2">
-        <v>27</v>
-      </c>
-      <c r="C3" s="14">
-        <v>85.5</v>
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>29</v>
+      </c>
+      <c r="C3" s="12">
+        <v>123.5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>28</v>
-      </c>
-      <c r="C4" s="15">
-        <v>89.9</v>
+        <v>40</v>
+      </c>
+      <c r="C4" s="12">
+        <v>123.5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>29</v>
-      </c>
-      <c r="C5" s="15">
-        <v>89.9</v>
+        <v>41</v>
+      </c>
+      <c r="C5" s="12">
+        <v>123.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>27</v>
-      </c>
-      <c r="C6" s="14">
-        <v>85.5</v>
+        <v>36</v>
+      </c>
+      <c r="C6" s="12">
+        <v>233.9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3">
-        <v>28</v>
-      </c>
-      <c r="C7" s="15">
-        <v>89.9</v>
+        <v>37</v>
+      </c>
+      <c r="C7" s="12">
+        <v>233.9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3">
-        <v>29</v>
-      </c>
-      <c r="C8" s="15">
-        <v>89.9</v>
+        <v>38</v>
+      </c>
+      <c r="C8" s="12">
+        <v>233.9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3">
-        <v>27</v>
-      </c>
-      <c r="C9" s="14">
-        <v>85.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3">
-        <v>28</v>
-      </c>
-      <c r="C10" s="15">
-        <v>89.9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="3">
-        <v>29</v>
-      </c>
-      <c r="C11" s="15">
-        <v>89.9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="3">
-        <v>29</v>
-      </c>
-      <c r="C12" s="15">
-        <v>123.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="3">
-        <v>40</v>
-      </c>
-      <c r="C13" s="15">
-        <v>123.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="3">
-        <v>41</v>
-      </c>
-      <c r="C14" s="15">
-        <v>123.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="3">
-        <v>36</v>
-      </c>
-      <c r="C15" s="15">
-        <v>233.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="3">
+        <v>42</v>
+      </c>
+      <c r="C9" s="12">
+        <v>99.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4">
         <v>37</v>
       </c>
-      <c r="C16" s="15">
-        <v>233.9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="3">
-        <v>38</v>
-      </c>
-      <c r="C17" s="15">
-        <v>233.9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="3">
-        <v>42</v>
-      </c>
-      <c r="C18" s="15">
+      <c r="C10" s="13">
         <v>99.99</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="4">
-        <v>37</v>
-      </c>
-      <c r="C19" s="16">
-        <v>99.99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="18" t="s">
+    <row r="11" spans="1:3" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="13">
-        <f>SUM(C3:C19)</f>
-        <v>2068.0800000000004</v>
+      <c r="B11" s="19"/>
+      <c r="C11" s="10">
+        <f>SUM(C3:C10)</f>
+        <v>1272.18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A11:B11"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6CF0F7-701F-4AD3-A160-66200CB65652}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>27</v>
+      </c>
+      <c r="C3" s="11">
+        <v>85.5</v>
+      </c>
+      <c r="D3" s="11">
+        <f>C3*$C$13</f>
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="11">
+        <f>(C3-D3)*E3</f>
+        <v>153.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
+        <v>28</v>
+      </c>
+      <c r="C4" s="12">
+        <v>89.9</v>
+      </c>
+      <c r="D4" s="11">
+        <f t="shared" ref="D4:D11" si="0">C4*$C$13</f>
+        <v>8.99</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3</v>
+      </c>
+      <c r="F4" s="11">
+        <f>C4*E4</f>
+        <v>269.70000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3">
+        <v>29</v>
+      </c>
+      <c r="C5" s="12">
+        <v>89.9</v>
+      </c>
+      <c r="D5" s="11">
+        <f t="shared" si="0"/>
+        <v>8.99</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="11">
+        <f>C5*E5</f>
+        <v>89.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3">
+        <v>27</v>
+      </c>
+      <c r="C6" s="11">
+        <v>85.5</v>
+      </c>
+      <c r="D6" s="11">
+        <f t="shared" si="0"/>
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="E6" s="3">
+        <v>5</v>
+      </c>
+      <c r="F6" s="11">
+        <f>C6*E6</f>
+        <v>427.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>28</v>
+      </c>
+      <c r="C7" s="12">
+        <v>89.9</v>
+      </c>
+      <c r="D7" s="11">
+        <f t="shared" si="0"/>
+        <v>8.99</v>
+      </c>
+      <c r="E7" s="3">
+        <v>3</v>
+      </c>
+      <c r="F7" s="11">
+        <f>C7*E7</f>
+        <v>269.70000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <v>29</v>
+      </c>
+      <c r="C8" s="12">
+        <v>89.9</v>
+      </c>
+      <c r="D8" s="11">
+        <f t="shared" si="0"/>
+        <v>8.99</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3</v>
+      </c>
+      <c r="F8" s="11">
+        <f>C8*E8</f>
+        <v>269.70000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3">
+        <v>27</v>
+      </c>
+      <c r="C9" s="11">
+        <v>85.5</v>
+      </c>
+      <c r="D9" s="11">
+        <f t="shared" si="0"/>
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="11">
+        <f>C9*E9</f>
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3">
+        <v>28</v>
+      </c>
+      <c r="C10" s="12">
+        <v>89.9</v>
+      </c>
+      <c r="D10" s="11">
+        <f t="shared" si="0"/>
+        <v>8.99</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2</v>
+      </c>
+      <c r="F10" s="11">
+        <f>C10*E10</f>
+        <v>179.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3">
+        <v>29</v>
+      </c>
+      <c r="C11" s="12">
+        <v>89.9</v>
+      </c>
+      <c r="D11" s="11">
+        <f t="shared" si="0"/>
+        <v>8.99</v>
+      </c>
+      <c r="E11" s="3">
+        <v>3</v>
+      </c>
+      <c r="F11" s="11">
+        <f>C11*E11</f>
+        <v>269.70000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="19"/>
+      <c r="C12" s="10">
+        <f>SUM(C3:C11)</f>
+        <v>795.9</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="14">
+        <f>E3+E4+E5+E6+E7+E8+E9+E10+E11</f>
+        <v>23</v>
+      </c>
+      <c r="F12" s="10">
+        <f>SUM(F3:F11)</f>
+        <v>2015.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:F13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>